<commit_message>
[ADD] Api test for advertisement
</commit_message>
<xml_diff>
--- a/Test case document - Advertisement.xlsx
+++ b/Test case document - Advertisement.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anjomathew/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anjomathew/projectAdvertisement/projectAdvertisement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B5C13A8-1F9C-0542-B6AC-9CA03DA96087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539886DE-6E1B-5248-8424-B80002DF5E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41720" yWindow="3440" windowWidth="34700" windowHeight="20520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Ui test cases" sheetId="1" r:id="rId1"/>
+    <sheet name="Api test cases" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="44">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -70,9 +71,6 @@
   </si>
   <si>
     <t>Test suite</t>
-  </si>
-  <si>
-    <t>Advertisment</t>
   </si>
   <si>
     <t>Save button is disabled if mandatory fields are not filled in add advertisement form</t>
@@ -127,10 +125,48 @@
     <t>User is abke to add a advertisement with all fields and all added fields are displayed in advertisement display list</t>
   </si>
   <si>
-    <t>Adv_1.0</t>
-  </si>
-  <si>
     <t>FAIL</t>
+  </si>
+  <si>
+    <t>Advertisment Ui test suite</t>
+  </si>
+  <si>
+    <t>ADV_UI_1.0</t>
+  </si>
+  <si>
+    <t>ADV_API_1.0</t>
+  </si>
+  <si>
+    <t>Advertisment Api test Suite</t>
+  </si>
+  <si>
+    <t>User is able to add advertisement with POST request</t>
+  </si>
+  <si>
+    <t>User is able to edit advertisement with PATCH request</t>
+  </si>
+  <si>
+    <t>User is able to edit advertisement with PUT request</t>
+  </si>
+  <si>
+    <t>User is able to get list of all advertisement with GET request</t>
+  </si>
+  <si>
+    <t>Error is shown in response if mandatory fields are missing from request body for POST request</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error code "404" is shown if incorrect request url is send for any method
+</t>
+  </si>
+  <si>
+    <t>User is able to get info about specific advertisement with GET request</t>
+  </si>
+  <si>
+    <t>Error is not shown if user sends a put request without whole body.
+Mandatory parameter like name and price</t>
+  </si>
+  <si>
+    <t>Error is shown if user passes _id in body for put request</t>
   </si>
 </sst>
 </file>
@@ -360,7 +396,109 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="20">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -707,7 +845,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
@@ -728,14 +866,14 @@
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="13"/>
       <c r="G2" s="14" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
@@ -807,7 +945,7 @@
       </c>
       <c r="F6" s="19"/>
       <c r="G6" s="20">
-        <v>44856</v>
+        <v>44795</v>
       </c>
       <c r="H6" s="21"/>
       <c r="I6" s="16" t="s">
@@ -815,7 +953,7 @@
       </c>
       <c r="J6" s="19"/>
       <c r="K6" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L6" s="10"/>
     </row>
@@ -828,7 +966,7 @@
       </c>
       <c r="D11" s="23"/>
       <c r="E11" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="23"/>
@@ -846,7 +984,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D13" s="25"/>
       <c r="E13" s="9" t="s">
@@ -860,7 +998,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="9" t="s">
@@ -874,7 +1012,7 @@
         <v>3</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="9" t="s">
@@ -888,7 +1026,7 @@
         <v>4</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="9" t="s">
@@ -902,7 +1040,7 @@
         <v>5</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="9" t="s">
@@ -916,7 +1054,7 @@
         <v>6</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="9" t="s">
@@ -930,7 +1068,7 @@
         <v>7</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="9" t="s">
@@ -944,7 +1082,7 @@
         <v>8</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="9" t="s">
@@ -958,7 +1096,7 @@
         <v>9</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="9" t="s">
@@ -972,7 +1110,7 @@
         <v>10</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="9" t="s">
@@ -986,7 +1124,7 @@
         <v>11</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="9" t="s">
@@ -1000,7 +1138,7 @@
         <v>12</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D24" s="8"/>
       <c r="E24" s="9" t="s">
@@ -1014,7 +1152,7 @@
         <v>13</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D25" s="8"/>
       <c r="E25" s="9" t="s">
@@ -1028,7 +1166,7 @@
         <v>14</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D26" s="8"/>
       <c r="E26" s="9" t="s">
@@ -1042,7 +1180,7 @@
         <v>15</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D27" s="8"/>
       <c r="E27" s="9" t="s">
@@ -1056,7 +1194,7 @@
         <v>16</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="9" t="s">
@@ -1117,30 +1255,30 @@
     <mergeCell ref="E26:G26"/>
   </mergeCells>
   <conditionalFormatting sqref="E13:G28">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="5" operator="equal">
       <formula>"Suspended"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="6" operator="equal">
       <formula>"Not Executed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="7" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="8" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:L6">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
       <formula>"Suspended"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
       <formula>"Not Executed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1152,4 +1290,365 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD1BBFFD-FEB5-4649-BEC1-D7A2D7B68A47}">
+  <dimension ref="B2:L28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="3" width="9.1640625" style="2"/>
+    <col min="4" max="4" width="49" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" style="2"/>
+    <col min="6" max="6" width="16.1640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" style="2"/>
+    <col min="8" max="8" width="30.5" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="9.1640625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="13"/>
+      <c r="G2" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="15"/>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="13"/>
+      <c r="G3" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="15"/>
+      <c r="I3" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="13"/>
+      <c r="K3" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="18"/>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="2:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="B6" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="19"/>
+      <c r="D6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="19"/>
+      <c r="G6" s="20">
+        <v>44795</v>
+      </c>
+      <c r="H6" s="21"/>
+      <c r="I6" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="19"/>
+      <c r="K6" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" s="10"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="23"/>
+      <c r="E11" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+    </row>
+    <row r="12" spans="2:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="23"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+    </row>
+    <row r="13" spans="2:12" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="6">
+        <v>1</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="25"/>
+      <c r="E13" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="10"/>
+      <c r="G13" s="11"/>
+    </row>
+    <row r="14" spans="2:12" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="6">
+        <v>2</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="10"/>
+      <c r="G14" s="11"/>
+    </row>
+    <row r="15" spans="2:12" ht="78.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="6">
+        <v>3</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="10"/>
+      <c r="G15" s="11"/>
+    </row>
+    <row r="16" spans="2:12" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="6">
+        <v>4</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="10"/>
+      <c r="G16" s="11"/>
+    </row>
+    <row r="17" spans="2:7" ht="104.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="6">
+        <v>5</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="8"/>
+      <c r="E17" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="10"/>
+      <c r="G17" s="11"/>
+    </row>
+    <row r="18" spans="2:7" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="6">
+        <v>6</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="8"/>
+      <c r="E18" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="10"/>
+      <c r="G18" s="11"/>
+    </row>
+    <row r="19" spans="2:7" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="6">
+        <v>7</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="10"/>
+      <c r="G19" s="11"/>
+    </row>
+    <row r="20" spans="2:7" ht="93" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="6">
+        <v>8</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="8"/>
+      <c r="E20" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="10"/>
+      <c r="G20" s="11"/>
+    </row>
+    <row r="21" spans="2:7" ht="83" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="6">
+        <v>9</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="10"/>
+      <c r="G21" s="11"/>
+    </row>
+    <row r="22" spans="2:7" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="6">
+        <v>10</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="8"/>
+      <c r="E22" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="10"/>
+      <c r="G22" s="11"/>
+    </row>
+    <row r="23" spans="2:7" ht="70" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="2:7" ht="70" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="2:7" ht="98" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="2:7" ht="67" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="2:7" ht="75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="2:7" ht="74" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <mergeCells count="36">
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:D12"/>
+    <mergeCell ref="E11:G12"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:L2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:G21"/>
+  </mergeCells>
+  <conditionalFormatting sqref="E13:G22">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+      <formula>"Suspended"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
+      <formula>"Not Executed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="8" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K6:L6">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+      <formula>"Suspended"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+      <formula>"Not Executed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E13:G22" xr:uid="{9A5428A4-6ECB-BE4E-BF97-32B32ECA8846}">
+      <formula1>"Pass, Fail, Not Executed, Suspended"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>